<commit_message>
feat: Apache POI ile Excel'e test sonuclari (PASSED/FAILED) yazdirma islemi basariyla eklendi
</commit_message>
<xml_diff>
--- a/src/test/resources/amazon_data.xlsx
+++ b/src/test/resources/amazon_data.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>AranacakKelime</t>
   </si>
@@ -49,12 +49,22 @@
   </si>
   <si>
     <t>Sensör</t>
+  </si>
+  <si>
+    <t>Test Sonucu</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>FAILED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -400,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -409,42 +419,51 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>2</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>3</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>5</v>
       </c>
     </row>

</xml_diff>